<commit_message>
Updated/removed phasome it output summaries and stats
</commit_message>
<xml_diff>
--- a/PhasomeIt_data/phasomeit_out_RNAcheck.xlsx
+++ b/PhasomeIt_data/phasomeit_out_RNAcheck.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u5501917/Documents/PhD/PhD/PhasomeIt_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390FFBD2-4D08-BF4C-A293-1C52B02D2D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF382DCA-EB62-D34D-916B-3C1FCAF46220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="760" windowWidth="15200" windowHeight="18880" firstSheet="3" activeTab="4" xr2:uid="{480DD372-3942-D34A-8BED-516D6EDEA6F5}"/>
+    <workbookView xWindow="200" yWindow="2800" windowWidth="15200" windowHeight="18880" firstSheet="3" activeTab="4" xr2:uid="{480DD372-3942-D34A-8BED-516D6EDEA6F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="9" r:id="rId1"/>
@@ -21487,9 +21487,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F7BEF31-A977-9C4C-B5E8-9BA5B0A6F49B}">
   <dimension ref="A1:AZ70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="112" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="92" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AC34" sqref="AC34"/>
+      <selection pane="topRight" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>